<commit_message>
commit pyscript update 4
1.增加timeout
2.增加token,数据表增加参数savetoken
3.增加环境变量，可配置可不配置,ON,启用环境参数
4.excel数据处理json
</commit_message>
<xml_diff>
--- a/API_py_scripts_debug/datadir/myapidata.xlsx
+++ b/API_py_scripts_debug/datadir/myapidata.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B0B426-473D-4F5F-80DC-7D0E9694AF94}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,80 +66,99 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>/farmplantend/plantUserWallet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{ "errno" : 0, "errmsg" : null, "data" : "" }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bdh获取钱包余额</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/farmplantend/farmlands/count</t>
+  </si>
+  <si>
+    <t>根据id获取地块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>application/x-www-form-urlencoded</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dev01.bdhlan.com:8080/bdhsystem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据i获取验证码d获取地块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/farmplantend/plantUser/checkCode</t>
+  </si>
+  <si>
+    <t>ip=192.168.1.17&amp;mobilePhone=15701137117</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>amount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B94ftK1WY6JSUe7hBTfmgOsGckPFbW8dRASuVNQ52ag5f9pS//4V5E66NZNgQq9tnw2GwdcnZgG7Nz6SEv/klZB+VHjS3DzMCKDb92L</t>
+  </si>
+  <si>
+    <t>bdh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bdh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dev01.bdhlan.com:8080/bdhsystem</t>
+  </si>
+  <si>
     <t>BDHAuthorization</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/farmplantend/plantUserWallet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> dev01.bdhlan.com:8080/bdhsystem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>method</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>get</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{ "errno" : 0, "errmsg" : null, "data" : "" }</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bdh获取钱包余额</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/farmplantend/farmlands/count</t>
-  </si>
-  <si>
-    <t>根据id获取地块</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>application/x-www-form-urlencoded</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>get</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dev01.bdhlan.com:8080/bdhsystem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>根据i获取验证码d获取地块</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/farmplantend/plantUser/checkCode</t>
-  </si>
-  <si>
-    <t>ip=192.168.1.17&amp;mobilePhone=15701137117</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>amount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B94ftK1WY6JSUe7hBTfmgOsGckPFbW8dRASuVNQ52ag5f9pS//4V5E66NZNgQq9tnw2GwdcnZgG7Nz6SEv/klZB+VHjS3DzMCKDb92L</t>
+    <t>savetoken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>header_data_token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>param_location_datas_data_token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,7 +257,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -274,7 +292,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -451,36 +469,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="16.25" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="22.625" customWidth="1"/>
-    <col min="5" max="5" width="10.875" customWidth="1"/>
-    <col min="6" max="6" width="5.125" customWidth="1"/>
-    <col min="7" max="7" width="7.125" customWidth="1"/>
-    <col min="8" max="8" width="12.625" customWidth="1"/>
-    <col min="10" max="10" width="12.875" customWidth="1"/>
-    <col min="11" max="11" width="17.75" customWidth="1"/>
-    <col min="12" max="12" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="13.25" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
+    <col min="5" max="5" width="8.25" customWidth="1"/>
+    <col min="6" max="6" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="7.875" customWidth="1"/>
+    <col min="8" max="8" width="14.625" customWidth="1"/>
+    <col min="9" max="9" width="11.625" customWidth="1"/>
+    <col min="10" max="10" width="8.875" customWidth="1"/>
+    <col min="11" max="11" width="17.875" customWidth="1"/>
+    <col min="12" max="12" width="21.875" customWidth="1"/>
+    <col min="13" max="13" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +514,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -517,57 +537,66 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
       <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
         <v>26</v>
       </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
+      <c r="M2" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="M3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -578,21 +607,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400E59C3-8DE3-48BD-BEAC-6FDDF917E956}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="7" max="7" width="8.75" customWidth="1"/>
     <col min="8" max="8" width="33.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +635,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -630,34 +659,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>